<commit_message>
Brought model up to version 2.1.1
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Costs.xlsx
+++ b/InputData/ccs/CC/CCS Costs.xlsx
@@ -1,46 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\ccs\CC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03285C26-06C0-4B28-9ED1-5B146403E504}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24915" windowHeight="13860"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="Calculations" sheetId="3" r:id="rId3"/>
-    <sheet name="Conversion Factors" sheetId="9" r:id="rId4"/>
-    <sheet name="India Estimates" sheetId="8" r:id="rId5"/>
-    <sheet name="Calcs" sheetId="7" r:id="rId6"/>
-    <sheet name="CC-CCoEtSOToCpY" sheetId="4" r:id="rId7"/>
-    <sheet name="CC-TOMCpTS" sheetId="5" r:id="rId8"/>
-    <sheet name="CC-EUpTCS" sheetId="6" r:id="rId9"/>
+    <sheet name="CC-CCoEtSOToCpY" sheetId="4" r:id="rId4"/>
+    <sheet name="CC-TOMCpTS" sheetId="5" r:id="rId5"/>
+    <sheet name="CC-EUpTCS" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
   <si>
     <t>Source:</t>
   </si>
   <si>
+    <t>David, Jeremy and Howard Herzog</t>
+  </si>
+  <si>
+    <t>The Cost of Carbon Capture</t>
+  </si>
+  <si>
+    <t>http://sequestration.mit.edu/pdf/David_and_Herzog.pdf</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
     <t>Input</t>
   </si>
   <si>
@@ -143,6 +143,24 @@
     <t>This is a copy of Table 2 from Herzog and David, "The Cost of Carbon Capture"</t>
   </si>
   <si>
+    <t>We are using 2012 values, not 2000 values, from the table.</t>
+  </si>
+  <si>
+    <t>Key to Table 2 Terms</t>
+  </si>
+  <si>
+    <t>IGCC = Integrated coal Gasification Combined Cycle</t>
+  </si>
+  <si>
+    <t>PC = Pulverized Coal</t>
+  </si>
+  <si>
+    <t>NGCC = Natural Gas Combined Cycle</t>
+  </si>
+  <si>
+    <t>mill = 1/1000th of a dollar, or 1/10th of a cent</t>
+  </si>
+  <si>
     <t>Industry (NGCC)</t>
   </si>
   <si>
@@ -179,31 +197,52 @@
     <t>CC Energy Use per Ton CO2 Sequestered</t>
   </si>
   <si>
+    <t>unknown (sometime after 2012)</t>
+  </si>
+  <si>
     <t>Notes:</t>
   </si>
   <si>
+    <t>As noted in the source paper, the "incremental" costs here refer to the costs associated with CCS,</t>
+  </si>
+  <si>
+    <t>additional to the costs of a similar power plant without CCS.</t>
+  </si>
+  <si>
     <t>electricity sector</t>
   </si>
   <si>
     <t>industry sector</t>
   </si>
   <si>
+    <t>We use IGCC to represent electric utilities (which are likely to primarily apply CCS to coal</t>
+  </si>
+  <si>
+    <t>plants) and NGCC to represent industry.</t>
+  </si>
+  <si>
     <t>CC Capital Cost of Eqpt to Sequester One Ton of CO2 per Year</t>
   </si>
   <si>
-    <t>Capital cost ($/(ton*yr))</t>
-  </si>
-  <si>
     <t>Capital Cost of Eqpt to Sequester One Ton of CO2 per Year</t>
   </si>
   <si>
-    <t>O&amp;M Cost per Ton ($/ton)</t>
-  </si>
-  <si>
     <t>RESULT ($/ton)</t>
   </si>
   <si>
-    <t>Energy Use per Ton Sequestered (BTU/ton)</t>
+    <t>The document does not specify the year of the dollars shown, so we assume that the</t>
+  </si>
+  <si>
+    <t>dollars (at least for the 2012 values) are in 2012 dollars and thus need no conversion.</t>
+  </si>
+  <si>
+    <t>Capital cost ($/(metric ton CO2e*yr))</t>
+  </si>
+  <si>
+    <t>O&amp;M Cost per Ton ($/metric ton CO2e)</t>
+  </si>
+  <si>
+    <t>Energy Use per Ton Sequestered (BTU/metric ton CO2e)</t>
   </si>
   <si>
     <t xml:space="preserve">This variable captures the capital and O&amp;M costs and energy use of </t>
@@ -213,216 +252,17 @@
   </si>
   <si>
     <t>sectors.</t>
-  </si>
-  <si>
-    <t>https://www.irade.org/website%20documents/CCS_IRAde_DST.pdf</t>
-  </si>
-  <si>
-    <t>Page 25</t>
-  </si>
-  <si>
-    <t>Analysis of Carbon Capture and Storage (CCS) Technology in the Context of Indian Power Sector</t>
-  </si>
-  <si>
-    <t>Jyoti Parikh (IRADe)</t>
-  </si>
-  <si>
-    <t>Cost Implications of Carbon Capture and Storage for the Coal Power Plants in India</t>
-  </si>
-  <si>
-    <t>https://www.sciencedirect.com/science/article/pii/S187661021401162X</t>
-  </si>
-  <si>
-    <t>Rao and Kumar</t>
-  </si>
-  <si>
-    <t>Energy Procedia   54  ( 2014 )  431 – 438, Page 436, Table 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generation costs for 4 plant cases. However this study does not mention the underlying capital </t>
-  </si>
-  <si>
-    <t>and O&amp;M costs for the incremental retrofit of the coal plants. Hence we use the existing US source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The only India source with plant-specific analysis is a 2014 study (Rao, Kumar) which estimates incremental </t>
-  </si>
-  <si>
-    <t>An older Indian study (IRADe) estimates the capital and O&amp;M costs based on esimates</t>
-  </si>
-  <si>
-    <t>Supercritical PC with
-MEA based CCS</t>
-  </si>
-  <si>
-    <t>Supercritical PC with
-CCS+OFC</t>
-  </si>
-  <si>
-    <t>Cost in 2016 INR</t>
-  </si>
-  <si>
-    <t>CO2 avoidance cost ₹/tonne</t>
-  </si>
-  <si>
-    <t>Averages</t>
-  </si>
-  <si>
-    <t>Table 6.1 Selected Clean Coal Technologies used in the IRADe’s India Technology Assessment Model</t>
-  </si>
-  <si>
-    <t>capital cost (₹/MW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O&amp;M ₹/MW </t>
-  </si>
-  <si>
-    <t>O&amp;M ₹/MW</t>
-  </si>
-  <si>
-    <t>% of CO2 avoidance cost from O&amp;M</t>
-  </si>
-  <si>
-    <t>O&amp;M cost per ton CO2 avoided</t>
-  </si>
-  <si>
-    <t>Cap cost per ton CO2 avoided</t>
-  </si>
-  <si>
-    <t>2016 INR</t>
-  </si>
-  <si>
-    <t>(from Table 5.13)</t>
-  </si>
-  <si>
-    <t>Specific fuel consumption
-(kg/kWh)</t>
-  </si>
-  <si>
-    <t>Electricity</t>
-  </si>
-  <si>
-    <t>India sources - Public</t>
-  </si>
-  <si>
-    <t>of global demonstration plants. Both sources are listed above</t>
-  </si>
-  <si>
-    <t>In the absence of India-specific, publicly available costs, we consulted with modellers at IRADe,</t>
-  </si>
-  <si>
-    <t>which is a member of the "Global Technology Watch Group on Advanced Clean Coal Technologies".</t>
-  </si>
-  <si>
-    <t>This group was constituted to develop a "Coal Road Map for India", by the Dept. of Science &amp;</t>
-  </si>
-  <si>
-    <t>Technology (DST) of the Govt. of India (Sanction No. DST/SPLICE/CCP/GTWG-02/2013(G) dated 01/09/2014).</t>
-  </si>
-  <si>
-    <t>In this study, coal-based technologies are assessed for India-specific conditions. Even though</t>
-  </si>
-  <si>
-    <t>the study is not available in the public domain, we refer to the India-specific estimates here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In India-specific CCS literature, natural gas based technologies rarely find mention. </t>
-  </si>
-  <si>
-    <t>Further, India's natural gas consumption has been largely reliant on imports, and we</t>
-  </si>
-  <si>
-    <t>don't think it would be feasible to use NGCC technologies. Hence, we retain the estimates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">as the specific consumption of coal and heat rates for India can be very different from US values. </t>
-  </si>
-  <si>
-    <r>
-      <t>The tables that are referred to in the study are provided in the</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 'India Estimates'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tab.</t>
-    </r>
-  </si>
-  <si>
-    <t>from coal-based CCS technologies from the electricity sector for industry as well.</t>
-  </si>
-  <si>
-    <t>India studies - Public</t>
-  </si>
-  <si>
-    <t>India estimates by IRADe used for the variable</t>
-  </si>
-  <si>
-    <t>Global Technology Watch Group on Advanced Clean Coal Technologies/
-Department of Science &amp; Technology</t>
-  </si>
-  <si>
-    <t>Coal Road Map for India</t>
-  </si>
-  <si>
-    <t>IRADe, IIT Delhi, IIT Bombay, IIT Madras</t>
-  </si>
-  <si>
-    <t>Source tables in 'India Estimates' tab</t>
-  </si>
-  <si>
-    <t>Ruppees per dollar</t>
-  </si>
-  <si>
-    <t>See scaling-factors.xlsx for source info</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Multiply by to get 2012 Dollars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD CPI </t>
-  </si>
-  <si>
-    <t>See cpi.xlsx for source info</t>
-  </si>
-  <si>
-    <t>2016 USD</t>
-  </si>
-  <si>
-    <t>2012 USD</t>
-  </si>
-  <si>
-    <t>(Table 6.1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,16 +300,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,20 +314,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -583,54 +403,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -660,47 +439,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -718,143 +466,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>67365</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>143630</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{500AF3EA-3BEC-469E-BCD9-E92CCD6B615C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2733675"/>
-          <a:ext cx="4944165" cy="5410955"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>172645</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19611</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD5B064F-DD9D-483C-AB00-49B8592E2092}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5019675" y="0"/>
-          <a:ext cx="8564170" cy="4020111"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>291811</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40998E3F-F074-44C9-B0DF-431AF8C1DD3F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="66675" y="47625"/>
-          <a:ext cx="3882736" cy="2533650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -933,23 +544,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -985,23 +579,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1177,249 +754,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="84.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="31">
-        <v>2018</v>
-      </c>
-      <c r="D7" s="31">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="2" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="31">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{8874C90D-5C9A-44D6-9C36-0F1BAA7CABAA}"/>
-    <hyperlink ref="D15" r:id="rId2" xr:uid="{AA83E611-79DE-414D-AC06-55715AB9E489}"/>
+    <hyperlink ref="B8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1434,36 +918,36 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="10">
         <v>2000</v>
@@ -1486,7 +970,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1500,7 +984,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" s="16">
         <v>1401</v>
@@ -1523,7 +1007,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" s="16">
         <v>7.9</v>
@@ -1546,7 +1030,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B8" s="16">
         <v>8081</v>
@@ -1569,7 +1053,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" s="16">
         <v>305</v>
@@ -1592,7 +1076,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B10" s="16">
         <v>2.65</v>
@@ -1615,7 +1099,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B11" s="16">
         <v>0.19400000000000001</v>
@@ -1638,7 +1122,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -1649,7 +1133,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B13" s="16">
         <v>6570</v>
@@ -1672,7 +1156,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B14" s="16">
         <v>15</v>
@@ -1695,7 +1179,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B15" s="16">
         <v>1.24</v>
@@ -1718,7 +1202,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B16" s="16">
         <v>90</v>
@@ -1741,7 +1225,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1752,7 +1236,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B18" s="16">
         <v>0.752</v>
@@ -1775,7 +1259,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B19" s="16">
         <v>32</v>
@@ -1798,7 +1282,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B20" s="16">
         <v>10</v>
@@ -1821,7 +1305,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B21" s="16">
         <v>7.9</v>
@@ -1844,7 +1328,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22" s="16">
         <v>4.99</v>
@@ -1867,7 +1351,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" s="16">
         <v>42.2</v>
@@ -1890,7 +1374,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -1901,7 +1385,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B25" s="16">
         <v>85.4</v>
@@ -1924,7 +1408,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B26" s="16">
         <v>9462</v>
@@ -1947,7 +1431,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B27" s="16">
         <v>1909</v>
@@ -1970,7 +1454,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B28" s="16">
         <v>8.7999999999999995E-2</v>
@@ -1993,7 +1477,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B29" s="16">
         <v>43.6</v>
@@ -2016,7 +1500,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B30" s="16">
         <v>11.7</v>
@@ -2039,7 +1523,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B31" s="16">
         <v>11.6</v>
@@ -2062,7 +1546,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B32" s="16">
         <v>6.69</v>
@@ -2085,7 +1569,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B33" s="16">
         <v>36.1</v>
@@ -2108,7 +1592,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -2119,7 +1603,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B35" s="16">
         <v>1.7</v>
@@ -2142,7 +1626,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B36" s="16">
         <v>14.6</v>
@@ -2165,7 +1649,7 @@
     </row>
     <row r="37" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B37" s="21">
         <v>26</v>
@@ -2192,12 +1676,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2208,7 +1690,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2216,15 +1698,15 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <f>'Table 2'!C9</f>
@@ -2237,7 +1719,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <f>'Table 2'!C13</f>
@@ -2250,7 +1732,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -2261,7 +1743,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B6" s="23">
         <f>B3/B4*B5</f>
@@ -2279,7 +1761,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2287,15 +1769,15 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <f>'Table 2'!C10</f>
@@ -2308,7 +1790,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>1E-3</v>
@@ -2319,7 +1801,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>1000</v>
@@ -2330,7 +1812,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B14" s="26">
         <f>B11*B12*B13</f>
@@ -2343,22 +1825,22 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <f>'Table 2'!C11</f>
@@ -2371,7 +1853,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>1000</v>
@@ -2382,7 +1864,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>3412</v>
@@ -2393,7 +1875,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <f>B19*B20*B21</f>
@@ -2410,57 +1892,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EF6D6A-CAEA-4466-8367-59ADEEC6827B}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
-        <v>2016</v>
-      </c>
-      <c r="B2" s="42">
-        <v>67.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2016</v>
-      </c>
-      <c r="B6" s="33">
-        <v>0.95661376543184151</v>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="28">
+        <f>Calculations!B6</f>
+        <v>41.856925418569254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="28">
+        <f>Calculations!C6</f>
+        <v>126.17960426179603</v>
       </c>
     </row>
   </sheetData>
@@ -2469,302 +1937,43 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21A2C14-1D85-4685-938F-DAD9ED607BBB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E80723D-912F-4B6D-BFE2-2D7E8918B54C}">
-  <dimension ref="A1:H21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="38">
-        <f>AVERAGE(1.06, 1.16)</f>
-        <v>1.1099999999999999</v>
-      </c>
-      <c r="H3" s="40" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="38">
-        <f>19*10^7</f>
-        <v>190000000</v>
-      </c>
-      <c r="C4" s="38">
-        <f>23*10^7</f>
-        <v>230000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="38">
-        <f>246*10^5</f>
-        <v>24600000</v>
-      </c>
-      <c r="C5" s="38">
-        <f>221*10^5</f>
-        <v>22100000</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="38">
-        <v>3736.04</v>
-      </c>
-      <c r="C6" s="38">
-        <v>3966.02</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7">
-        <f>1/G3</f>
-        <v>0.90090090090090102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8">
-        <v>1000</v>
-      </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="38">
-        <f>AVERAGE(B4:C4)</f>
-        <v>210000000</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9">
-        <v>3412</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="38">
-        <f>AVERAGE(B5:C5)</f>
-        <v>23350000</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="47">
-        <f>G7*G8*G9</f>
-        <v>3073873.8738738741</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="38">
-        <f t="shared" ref="B11" si="0">AVERAGE(B6:C6)</f>
-        <v>3851.0299999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="39">
-        <f>B10/B9</f>
-        <v>0.11119047619047619</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="39">
-        <f>B13*B11</f>
-        <v>428.19785952380948</v>
-      </c>
-      <c r="C14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="39">
-        <f>B11-B14</f>
-        <v>3422.83214047619</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="28">
-        <f>B14/'Conversion Factors'!B2</f>
-        <v>6.3016609201443634</v>
-      </c>
-      <c r="C17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="46">
-        <f>B17*'Conversion Factors'!B6</f>
-        <v>6.0282555812939824</v>
-      </c>
-      <c r="C18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="28">
-        <f>B15/'Conversion Factors'!B2</f>
-        <v>50.37280559935526</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="46">
-        <f>B20*'Conversion Factors'!B6</f>
-        <v>48.187319239765387</v>
-      </c>
-      <c r="C21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>50</v>
-      </c>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="28">
-        <f>Calcs!B21</f>
-        <v>48.187319239765387</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <f>Calculations!B14</f>
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="28">
-        <f>B2</f>
-        <v>48.187319239765387</v>
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <f>Calculations!C14</f>
+        <v>4.68</v>
       </c>
     </row>
   </sheetData>
@@ -2772,95 +1981,44 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="28">
-        <f>Calcs!B18</f>
-        <v>6.0282555812939824</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="28">
-        <f>B2</f>
-        <v>6.0282555812939824</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>46</v>
-      </c>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="34">
-        <f>Calcs!G10</f>
-        <v>3073873.8738738741</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <f>Calculations!B22</f>
+        <v>460620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="34">
-        <f>B2</f>
-        <v>3073873.8738738741</v>
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <f>Calculations!C22</f>
+        <v>1013364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edits incorporating files WRI sent 5/21/20
</commit_message>
<xml_diff>
--- a/InputData/ccs/CC/CCS Costs.xlsx
+++ b/InputData/ccs/CC/CCS Costs.xlsx
@@ -1,46 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\ccs\CC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\ccs\CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03285C26-06C0-4B28-9ED1-5B146403E504}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24915" windowHeight="13860"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="Calculations" sheetId="3" r:id="rId3"/>
-    <sheet name="CC-CCoEtSOToCpY" sheetId="4" r:id="rId4"/>
-    <sheet name="CC-TOMCpTS" sheetId="5" r:id="rId5"/>
-    <sheet name="CC-EUpTCS" sheetId="6" r:id="rId6"/>
+    <sheet name="Conversion Factors" sheetId="9" r:id="rId4"/>
+    <sheet name="India Estimates" sheetId="8" r:id="rId5"/>
+    <sheet name="Calcs" sheetId="7" r:id="rId6"/>
+    <sheet name="CC-CCoEtSOToCpY" sheetId="4" r:id="rId7"/>
+    <sheet name="CC-TOMCpTS" sheetId="5" r:id="rId8"/>
+    <sheet name="CC-EUpTCS" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
   <si>
     <t>Source:</t>
   </si>
   <si>
-    <t>David, Jeremy and Howard Herzog</t>
-  </si>
-  <si>
-    <t>The Cost of Carbon Capture</t>
-  </si>
-  <si>
-    <t>http://sequestration.mit.edu/pdf/David_and_Herzog.pdf</t>
-  </si>
-  <si>
-    <t>Table 2</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
@@ -143,24 +143,6 @@
     <t>This is a copy of Table 2 from Herzog and David, "The Cost of Carbon Capture"</t>
   </si>
   <si>
-    <t>We are using 2012 values, not 2000 values, from the table.</t>
-  </si>
-  <si>
-    <t>Key to Table 2 Terms</t>
-  </si>
-  <si>
-    <t>IGCC = Integrated coal Gasification Combined Cycle</t>
-  </si>
-  <si>
-    <t>PC = Pulverized Coal</t>
-  </si>
-  <si>
-    <t>NGCC = Natural Gas Combined Cycle</t>
-  </si>
-  <si>
-    <t>mill = 1/1000th of a dollar, or 1/10th of a cent</t>
-  </si>
-  <si>
     <t>Industry (NGCC)</t>
   </si>
   <si>
@@ -197,52 +179,31 @@
     <t>CC Energy Use per Ton CO2 Sequestered</t>
   </si>
   <si>
-    <t>unknown (sometime after 2012)</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
-    <t>As noted in the source paper, the "incremental" costs here refer to the costs associated with CCS,</t>
-  </si>
-  <si>
-    <t>additional to the costs of a similar power plant without CCS.</t>
-  </si>
-  <si>
     <t>electricity sector</t>
   </si>
   <si>
     <t>industry sector</t>
   </si>
   <si>
-    <t>We use IGCC to represent electric utilities (which are likely to primarily apply CCS to coal</t>
-  </si>
-  <si>
-    <t>plants) and NGCC to represent industry.</t>
-  </si>
-  <si>
     <t>CC Capital Cost of Eqpt to Sequester One Ton of CO2 per Year</t>
   </si>
   <si>
+    <t>Capital cost ($/(ton*yr))</t>
+  </si>
+  <si>
     <t>Capital Cost of Eqpt to Sequester One Ton of CO2 per Year</t>
   </si>
   <si>
+    <t>O&amp;M Cost per Ton ($/ton)</t>
+  </si>
+  <si>
     <t>RESULT ($/ton)</t>
   </si>
   <si>
-    <t>The document does not specify the year of the dollars shown, so we assume that the</t>
-  </si>
-  <si>
-    <t>dollars (at least for the 2012 values) are in 2012 dollars and thus need no conversion.</t>
-  </si>
-  <si>
-    <t>Capital cost ($/(metric ton CO2e*yr))</t>
-  </si>
-  <si>
-    <t>O&amp;M Cost per Ton ($/metric ton CO2e)</t>
-  </si>
-  <si>
-    <t>Energy Use per Ton Sequestered (BTU/metric ton CO2e)</t>
+    <t>Energy Use per Ton Sequestered (BTU/ton)</t>
   </si>
   <si>
     <t xml:space="preserve">This variable captures the capital and O&amp;M costs and energy use of </t>
@@ -252,17 +213,216 @@
   </si>
   <si>
     <t>sectors.</t>
+  </si>
+  <si>
+    <t>https://www.irade.org/website%20documents/CCS_IRAde_DST.pdf</t>
+  </si>
+  <si>
+    <t>Page 25</t>
+  </si>
+  <si>
+    <t>Analysis of Carbon Capture and Storage (CCS) Technology in the Context of Indian Power Sector</t>
+  </si>
+  <si>
+    <t>Jyoti Parikh (IRADe)</t>
+  </si>
+  <si>
+    <t>Cost Implications of Carbon Capture and Storage for the Coal Power Plants in India</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S187661021401162X</t>
+  </si>
+  <si>
+    <t>Rao and Kumar</t>
+  </si>
+  <si>
+    <t>Energy Procedia   54  ( 2014 )  431 – 438, Page 436, Table 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generation costs for 4 plant cases. However this study does not mention the underlying capital </t>
+  </si>
+  <si>
+    <t>and O&amp;M costs for the incremental retrofit of the coal plants. Hence we use the existing US source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The only India source with plant-specific analysis is a 2014 study (Rao, Kumar) which estimates incremental </t>
+  </si>
+  <si>
+    <t>An older Indian study (IRADe) estimates the capital and O&amp;M costs based on esimates</t>
+  </si>
+  <si>
+    <t>Supercritical PC with
+MEA based CCS</t>
+  </si>
+  <si>
+    <t>Supercritical PC with
+CCS+OFC</t>
+  </si>
+  <si>
+    <t>Cost in 2016 INR</t>
+  </si>
+  <si>
+    <t>CO2 avoidance cost ₹/tonne</t>
+  </si>
+  <si>
+    <t>Averages</t>
+  </si>
+  <si>
+    <t>Table 6.1 Selected Clean Coal Technologies used in the IRADe’s India Technology Assessment Model</t>
+  </si>
+  <si>
+    <t>capital cost (₹/MW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O&amp;M ₹/MW </t>
+  </si>
+  <si>
+    <t>O&amp;M ₹/MW</t>
+  </si>
+  <si>
+    <t>% of CO2 avoidance cost from O&amp;M</t>
+  </si>
+  <si>
+    <t>O&amp;M cost per ton CO2 avoided</t>
+  </si>
+  <si>
+    <t>Cap cost per ton CO2 avoided</t>
+  </si>
+  <si>
+    <t>2016 INR</t>
+  </si>
+  <si>
+    <t>(from Table 5.13)</t>
+  </si>
+  <si>
+    <t>Specific fuel consumption
+(kg/kWh)</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>India sources - Public</t>
+  </si>
+  <si>
+    <t>of global demonstration plants. Both sources are listed above</t>
+  </si>
+  <si>
+    <t>In the absence of India-specific, publicly available costs, we consulted with modellers at IRADe,</t>
+  </si>
+  <si>
+    <t>which is a member of the "Global Technology Watch Group on Advanced Clean Coal Technologies".</t>
+  </si>
+  <si>
+    <t>This group was constituted to develop a "Coal Road Map for India", by the Dept. of Science &amp;</t>
+  </si>
+  <si>
+    <t>Technology (DST) of the Govt. of India (Sanction No. DST/SPLICE/CCP/GTWG-02/2013(G) dated 01/09/2014).</t>
+  </si>
+  <si>
+    <t>In this study, coal-based technologies are assessed for India-specific conditions. Even though</t>
+  </si>
+  <si>
+    <t>the study is not available in the public domain, we refer to the India-specific estimates here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In India-specific CCS literature, natural gas based technologies rarely find mention. </t>
+  </si>
+  <si>
+    <t>Further, India's natural gas consumption has been largely reliant on imports, and we</t>
+  </si>
+  <si>
+    <t>don't think it would be feasible to use NGCC technologies. Hence, we retain the estimates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">as the specific consumption of coal and heat rates for India can be very different from US values. </t>
+  </si>
+  <si>
+    <r>
+      <t>The tables that are referred to in the study are provided in the</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'India Estimates'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab.</t>
+    </r>
+  </si>
+  <si>
+    <t>from coal-based CCS technologies from the electricity sector for industry as well.</t>
+  </si>
+  <si>
+    <t>India studies - Public</t>
+  </si>
+  <si>
+    <t>India estimates by IRADe used for the variable</t>
+  </si>
+  <si>
+    <t>Global Technology Watch Group on Advanced Clean Coal Technologies/
+Department of Science &amp; Technology</t>
+  </si>
+  <si>
+    <t>Coal Road Map for India</t>
+  </si>
+  <si>
+    <t>IRADe, IIT Delhi, IIT Bombay, IIT Madras</t>
+  </si>
+  <si>
+    <t>Source tables in 'India Estimates' tab</t>
+  </si>
+  <si>
+    <t>Ruppees per dollar</t>
+  </si>
+  <si>
+    <t>See scaling-factors.xlsx for source info</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Multiply by to get 2012 Dollars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD CPI </t>
+  </si>
+  <si>
+    <t>See cpi.xlsx for source info</t>
+  </si>
+  <si>
+    <t>2016 USD</t>
+  </si>
+  <si>
+    <t>2012 USD</t>
+  </si>
+  <si>
+    <t>(Table 6.1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +460,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,8 +482,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -403,13 +583,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -439,16 +660,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -466,6 +718,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>67365</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>143630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{500AF3EA-3BEC-469E-BCD9-E92CCD6B615C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2733675"/>
+          <a:ext cx="4944165" cy="5410955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>172645</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD5B064F-DD9D-483C-AB00-49B8592E2092}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5019675" y="0"/>
+          <a:ext cx="8564170" cy="4020111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>291811</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40998E3F-F074-44C9-B0DF-431AF8C1DD3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="47625"/>
+          <a:ext cx="3882736" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,6 +933,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -579,6 +985,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -754,156 +1177,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="84.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="31">
+        <v>2018</v>
+      </c>
+      <c r="D7" s="31">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="31">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>69</v>
-      </c>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="30"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="30"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{8874C90D-5C9A-44D6-9C36-0F1BAA7CABAA}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{AA83E611-79DE-414D-AC06-55715AB9E489}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -918,36 +1434,36 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="10">
         <v>2000</v>
@@ -970,7 +1486,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -984,7 +1500,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="16">
         <v>1401</v>
@@ -1007,7 +1523,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="16">
         <v>7.9</v>
@@ -1030,7 +1546,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="16">
         <v>8081</v>
@@ -1053,7 +1569,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" s="16">
         <v>305</v>
@@ -1076,7 +1592,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="16">
         <v>2.65</v>
@@ -1099,7 +1615,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" s="16">
         <v>0.19400000000000001</v>
@@ -1122,7 +1638,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -1133,7 +1649,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B13" s="16">
         <v>6570</v>
@@ -1156,7 +1672,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B14" s="16">
         <v>15</v>
@@ -1179,7 +1695,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" s="16">
         <v>1.24</v>
@@ -1202,7 +1718,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B16" s="16">
         <v>90</v>
@@ -1225,7 +1741,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1236,7 +1752,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B18" s="16">
         <v>0.752</v>
@@ -1259,7 +1775,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B19" s="16">
         <v>32</v>
@@ -1282,7 +1798,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20" s="16">
         <v>10</v>
@@ -1305,7 +1821,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B21" s="16">
         <v>7.9</v>
@@ -1328,7 +1844,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B22" s="16">
         <v>4.99</v>
@@ -1351,7 +1867,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B23" s="16">
         <v>42.2</v>
@@ -1374,7 +1890,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -1385,7 +1901,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B25" s="16">
         <v>85.4</v>
@@ -1408,7 +1924,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B26" s="16">
         <v>9462</v>
@@ -1431,7 +1947,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B27" s="16">
         <v>1909</v>
@@ -1454,7 +1970,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B28" s="16">
         <v>8.7999999999999995E-2</v>
@@ -1477,7 +1993,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B29" s="16">
         <v>43.6</v>
@@ -1500,7 +2016,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B30" s="16">
         <v>11.7</v>
@@ -1523,7 +2039,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B31" s="16">
         <v>11.6</v>
@@ -1546,7 +2062,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B32" s="16">
         <v>6.69</v>
@@ -1569,7 +2085,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B33" s="16">
         <v>36.1</v>
@@ -1592,7 +2108,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -1603,7 +2119,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B35" s="16">
         <v>1.7</v>
@@ -1626,7 +2142,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B36" s="16">
         <v>14.6</v>
@@ -1649,7 +2165,7 @@
     </row>
     <row r="37" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B37" s="21">
         <v>26</v>
@@ -1676,10 +2192,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1690,7 +2208,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1698,15 +2216,15 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <f>'Table 2'!C9</f>
@@ -1719,7 +2237,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <f>'Table 2'!C13</f>
@@ -1732,7 +2250,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -1743,7 +2261,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B6" s="23">
         <f>B3/B4*B5</f>
@@ -1761,7 +2279,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1769,15 +2287,15 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <f>'Table 2'!C10</f>
@@ -1790,7 +2308,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>1E-3</v>
@@ -1801,7 +2319,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>1000</v>
@@ -1812,7 +2330,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B14" s="26">
         <f>B11*B12*B13</f>
@@ -1825,22 +2343,22 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <f>'Table 2'!C11</f>
@@ -1853,7 +2371,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>1000</v>
@@ -1864,7 +2382,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>3412</v>
@@ -1875,7 +2393,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <f>B19*B20*B21</f>
@@ -1892,43 +2410,361 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EF6D6A-CAEA-4466-8367-59ADEEC6827B}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="42">
+        <v>2016</v>
+      </c>
+      <c r="B2" s="42">
+        <v>67.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0.95661376543184151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21A2C14-1D85-4685-938F-DAD9ED607BBB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E80723D-912F-4B6D-BFE2-2D7E8918B54C}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="36"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="38">
+        <f>AVERAGE(1.06, 1.16)</f>
+        <v>1.1099999999999999</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="38">
+        <f>19*10^7</f>
+        <v>190000000</v>
+      </c>
+      <c r="C4" s="38">
+        <f>23*10^7</f>
+        <v>230000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="38">
+        <f>246*10^5</f>
+        <v>24600000</v>
+      </c>
+      <c r="C5" s="38">
+        <f>221*10^5</f>
+        <v>22100000</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="38">
+        <v>3736.04</v>
+      </c>
+      <c r="C6" s="38">
+        <v>3966.02</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <f>1/G3</f>
+        <v>0.90090090090090102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="38">
+        <f>AVERAGE(B4:C4)</f>
+        <v>210000000</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>3412</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="38">
+        <f>AVERAGE(B5:C5)</f>
+        <v>23350000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="47">
+        <f>G7*G8*G9</f>
+        <v>3073873.8738738741</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="38">
+        <f t="shared" ref="B11" si="0">AVERAGE(B6:C6)</f>
+        <v>3851.0299999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="39">
+        <f>B10/B9</f>
+        <v>0.11119047619047619</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="39">
+        <f>B13*B11</f>
+        <v>428.19785952380948</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="39">
+        <f>B11-B14</f>
+        <v>3422.83214047619</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="28">
+        <f>B14/'Conversion Factors'!B2</f>
+        <v>6.3016609201443634</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="46">
+        <f>B17*'Conversion Factors'!B6</f>
+        <v>6.0282555812939824</v>
+      </c>
+      <c r="C18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="28">
+        <f>B15/'Conversion Factors'!B2</f>
+        <v>50.37280559935526</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="46">
+        <f>B20*'Conversion Factors'!B6</f>
+        <v>48.187319239765387</v>
+      </c>
+      <c r="C21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>50</v>
+      </c>
       <c r="B1" s="29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B2" s="28">
-        <f>Calculations!B6</f>
-        <v>41.856925418569254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <f>Calcs!B21</f>
+        <v>48.187319239765387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B3" s="28">
-        <f>Calculations!C6</f>
-        <v>126.17960426179603</v>
+        <f>B2</f>
+        <v>48.187319239765387</v>
       </c>
     </row>
   </sheetData>
@@ -1936,44 +2772,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>45</v>
+      </c>
       <c r="B1" s="29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2">
-        <f>Calculations!B14</f>
-        <v>2.39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="B2" s="28">
+        <f>Calcs!B18</f>
+        <v>6.0282555812939824</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
-        <f>Calculations!C14</f>
-        <v>4.68</v>
+        <v>49</v>
+      </c>
+      <c r="B3" s="28">
+        <f>B2</f>
+        <v>6.0282555812939824</v>
       </c>
     </row>
   </sheetData>
@@ -1981,44 +2820,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>46</v>
+      </c>
       <c r="B1" s="29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2">
-        <f>Calculations!B22</f>
-        <v>460620</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="B2" s="34">
+        <f>Calcs!G10</f>
+        <v>3073873.8738738741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
-        <f>Calculations!C22</f>
-        <v>1013364</v>
+        <v>49</v>
+      </c>
+      <c r="B3" s="34">
+        <f>B2</f>
+        <v>3073873.8738738741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>